<commit_message>
added benchmark data and some code rejigs
</commit_message>
<xml_diff>
--- a/documents/Benchmark Data.xlsx
+++ b/documents/Benchmark Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tudublin-my.sharepoint.com/personal/c20394933_mytudublin_ie/Documents/Year 4/cooper/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{367C46EC-07C1-4CCF-9584-CAD62B13634C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4BABDC0E-DE1B-48E4-B5B0-08A665A0BD00}"/>
+  <xr:revisionPtr revIDLastSave="157" documentId="8_{367C46EC-07C1-4CCF-9584-CAD62B13634C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7350C4F-F1F0-40A9-96C2-17840DFBB314}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="37710" windowHeight="21840" xr2:uid="{5475F6D4-1A11-4EC3-B7D0-BA9BA44DCB81}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="166">
   <si>
     <t>shadow_pass_0</t>
   </si>
@@ -519,6 +519,21 @@
   </si>
   <si>
     <t>2.4629997s</t>
+  </si>
+  <si>
+    <t>Insert</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>Insert (diverse)</t>
+  </si>
+  <si>
+    <t>Search (diverse)</t>
+  </si>
+  <si>
+    <t>ms</t>
   </si>
 </sst>
 </file>
@@ -562,9 +577,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2054,7 +2070,1926 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="107"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="7"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$66</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Insert</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:tint val="77000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$67:$A$84</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$67:$B$84</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>1.3883999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2861000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.2713999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.4257999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3492000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5346E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.1192000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.2285E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0505000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.11892999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.30330000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.59575</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.1859999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.1135999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.5065999999999997</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>13.281000000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>33.305999999999997</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>66.424999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A691-4C37-8353-4E70E11A06D6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$66</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Insert (diverse)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:shade val="76000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$67:$A$84</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$67:$C$84</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>6.2578E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.6773999999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8959E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.8518999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0942000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.7056000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.11684</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.22767999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.34097</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.44408999999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1285000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.2772999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.5782999999999996</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12.762</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>26.936</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>54.502000000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>134.22999999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>267.81</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A691-4C37-8353-4E70E11A06D6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1582640192"/>
+        <c:axId val="1582639712"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1582640192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1582639712"/>
+        <c:crossesAt val="1"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1582639712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1582640192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IE"/>
+              <a:t>Logaritmic</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-IE" baseline="0"/>
+              <a:t> Scale of  Time to Insert (no Entities to time taken to inser in ms)</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IE" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-IE"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$66</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Insert</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$67:$A$84</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$67:$B$84</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>1.3883999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2861000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.2713999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.4257999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3492000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5346E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.1192000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.2285E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0505000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.11892999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.30330000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.59575</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.1859999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.1135999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.5065999999999997</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>13.281000000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>33.305999999999997</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>66.424999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-493A-4AD9-BC1C-225D59C50CA6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$66</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Insert (diverse)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$67:$A$84</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$67:$C$84</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>6.2578E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.6773999999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8959E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.8518999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0942000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.7056000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.11684</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.22767999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.34097</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.44408999999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1285000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.2772999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.5782999999999996</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12.762</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>26.936</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>54.502000000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>134.22999999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>267.81</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-493A-4AD9-BC1C-225D59C50CA6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1587368944"/>
+        <c:axId val="1587366064"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1587368944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1587366064"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1587366064"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1587368944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IE" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Logaritmic Scale of  Time to Search(Entities to time taken to search in ms)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$66</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Search (diverse)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$G$67:$G$84</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$67:$H$84</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>1.9652999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0704999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1517000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.9627000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.615E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0966E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.8655000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.5312999999999995E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.3144999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.6854000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.8888E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.5693000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.5032E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.6923999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.3591000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.14702000000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.37046000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.73397000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9086-4A07-A9E7-E4EEEDCC2A59}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$66</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Search</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$G$67:$G$84</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$67:$I$84</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>1.6558999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6801000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7971E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0445000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.2327999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.7140999999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.9531000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.1733999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.5268E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.6202999999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.3971000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.6191999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.0701000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.2411999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.9092999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.9092999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.12266000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.25130999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9086-4A07-A9E7-E4EEEDCC2A59}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1038149216"/>
+        <c:axId val="1038150176"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1038149216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1038150176"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1038150176"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1038149216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinearReversed" id="25">
+  <a:schemeClr val="accent5"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2618,6 +4553,1515 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2651,6 +6095,114 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>1085850</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7DBB228-D006-A13C-5EDD-82E37CCB1748}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>100012</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>966787</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94125236-DC60-E04B-91DE-66668A01E0FB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>519112</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>195262</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{868182A3-B96E-0476-B387-7988643981E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2976,16 +6528,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00BBE059-4113-4126-B80E-773F440894EF}">
-  <dimension ref="A1:V60"/>
+  <dimension ref="A1:V84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59:B60"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U72" sqref="U72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17.85546875" bestFit="1" customWidth="1"/>
@@ -4601,6 +8153,383 @@
         <v>160</v>
       </c>
     </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>165</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>10</v>
+      </c>
+      <c r="B67" s="2">
+        <v>1.3883999999999999E-3</v>
+      </c>
+      <c r="C67" s="2">
+        <v>6.2578E-3</v>
+      </c>
+      <c r="G67" s="1">
+        <v>10</v>
+      </c>
+      <c r="H67">
+        <v>1.9652999999999999E-4</v>
+      </c>
+      <c r="I67">
+        <v>1.6558999999999999E-4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>20</v>
+      </c>
+      <c r="B68" s="2">
+        <v>2.2861000000000001E-3</v>
+      </c>
+      <c r="C68" s="2">
+        <v>9.6773999999999992E-3</v>
+      </c>
+      <c r="G68" s="1">
+        <v>20</v>
+      </c>
+      <c r="H68">
+        <v>2.0704999999999999E-4</v>
+      </c>
+      <c r="I68">
+        <v>1.6801000000000001E-4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>50</v>
+      </c>
+      <c r="B69" s="2">
+        <v>4.2713999999999998E-3</v>
+      </c>
+      <c r="C69" s="2">
+        <v>1.8959E-2</v>
+      </c>
+      <c r="G69" s="1">
+        <v>50</v>
+      </c>
+      <c r="H69">
+        <v>1.1517000000000001E-3</v>
+      </c>
+      <c r="I69">
+        <v>1.7971E-4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>100</v>
+      </c>
+      <c r="B70" s="2">
+        <v>7.4257999999999998E-3</v>
+      </c>
+      <c r="C70" s="2">
+        <v>2.8518999999999999E-2</v>
+      </c>
+      <c r="G70" s="1">
+        <v>100</v>
+      </c>
+      <c r="H70">
+        <v>2.9627000000000001E-4</v>
+      </c>
+      <c r="I70">
+        <v>2.0445000000000001E-4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>200</v>
+      </c>
+      <c r="B71" s="2">
+        <v>1.3492000000000001E-2</v>
+      </c>
+      <c r="C71" s="2">
+        <v>5.0942000000000001E-2</v>
+      </c>
+      <c r="G71" s="1">
+        <v>200</v>
+      </c>
+      <c r="H71">
+        <v>3.615E-4</v>
+      </c>
+      <c r="I71">
+        <v>2.2327999999999999E-4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>400</v>
+      </c>
+      <c r="B72" s="2">
+        <v>2.5346E-2</v>
+      </c>
+      <c r="C72" s="2">
+        <v>9.7056000000000003E-2</v>
+      </c>
+      <c r="G72" s="1">
+        <v>400</v>
+      </c>
+      <c r="H72">
+        <v>5.0966E-4</v>
+      </c>
+      <c r="I72">
+        <v>2.7140999999999998E-4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>500</v>
+      </c>
+      <c r="B73" s="2">
+        <v>3.1192000000000001E-2</v>
+      </c>
+      <c r="C73" s="2">
+        <v>0.11684</v>
+      </c>
+      <c r="G73" s="1">
+        <v>500</v>
+      </c>
+      <c r="H73">
+        <v>5.8655000000000003E-4</v>
+      </c>
+      <c r="I73">
+        <v>2.9531000000000002E-4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B74" s="2">
+        <v>6.2285E-2</v>
+      </c>
+      <c r="C74" s="2">
+        <v>0.22767999999999999</v>
+      </c>
+      <c r="G74" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H74">
+        <v>9.5312999999999995E-4</v>
+      </c>
+      <c r="I74">
+        <v>4.1733999999999999E-4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>1500</v>
+      </c>
+      <c r="B75" s="2">
+        <v>9.0505000000000002E-2</v>
+      </c>
+      <c r="C75" s="2">
+        <v>0.34097</v>
+      </c>
+      <c r="G75" s="1">
+        <v>1500</v>
+      </c>
+      <c r="H75">
+        <v>1.3144999999999999E-3</v>
+      </c>
+      <c r="I75">
+        <v>1.5268E-3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B76" s="2">
+        <v>0.11892999999999999</v>
+      </c>
+      <c r="C76" s="2">
+        <v>0.44408999999999998</v>
+      </c>
+      <c r="G76" s="1">
+        <v>2000</v>
+      </c>
+      <c r="H76">
+        <v>1.6854000000000001E-3</v>
+      </c>
+      <c r="I76">
+        <v>6.6202999999999998E-4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>5000</v>
+      </c>
+      <c r="B77" s="2">
+        <v>0.30330000000000001</v>
+      </c>
+      <c r="C77" s="2">
+        <v>1.1285000000000001</v>
+      </c>
+      <c r="G77" s="1">
+        <v>5000</v>
+      </c>
+      <c r="H77">
+        <v>3.8888E-3</v>
+      </c>
+      <c r="I77">
+        <v>1.3971000000000001E-3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>10000</v>
+      </c>
+      <c r="B78" s="2">
+        <v>0.59575</v>
+      </c>
+      <c r="C78" s="2">
+        <v>2.2772999999999999</v>
+      </c>
+      <c r="G78" s="1">
+        <v>10000</v>
+      </c>
+      <c r="H78">
+        <v>7.5693000000000002E-3</v>
+      </c>
+      <c r="I78">
+        <v>2.6191999999999999E-3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>20000</v>
+      </c>
+      <c r="B79" s="2">
+        <v>1.1859999999999999</v>
+      </c>
+      <c r="C79" s="2">
+        <v>4.5782999999999996</v>
+      </c>
+      <c r="G79" s="1">
+        <v>20000</v>
+      </c>
+      <c r="H79">
+        <v>1.5032E-2</v>
+      </c>
+      <c r="I79">
+        <v>5.0701000000000001E-3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>50000</v>
+      </c>
+      <c r="B80" s="2">
+        <v>3.1135999999999999</v>
+      </c>
+      <c r="C80" s="2">
+        <v>12.762</v>
+      </c>
+      <c r="G80" s="1">
+        <v>50000</v>
+      </c>
+      <c r="H80">
+        <v>3.6923999999999998E-2</v>
+      </c>
+      <c r="I80">
+        <v>1.2411999999999999E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>100000</v>
+      </c>
+      <c r="B81" s="2">
+        <v>6.5065999999999997</v>
+      </c>
+      <c r="C81" s="2">
+        <v>26.936</v>
+      </c>
+      <c r="G81" s="1">
+        <v>100000</v>
+      </c>
+      <c r="H81">
+        <v>7.3591000000000004E-2</v>
+      </c>
+      <c r="I81">
+        <v>4.9092999999999998E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>200000</v>
+      </c>
+      <c r="B82" s="2">
+        <v>13.281000000000001</v>
+      </c>
+      <c r="C82" s="2">
+        <v>54.502000000000002</v>
+      </c>
+      <c r="G82" s="1">
+        <v>200000</v>
+      </c>
+      <c r="H82">
+        <v>0.14702000000000001</v>
+      </c>
+      <c r="I82">
+        <v>4.9092999999999998E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>500000</v>
+      </c>
+      <c r="B83" s="2">
+        <v>33.305999999999997</v>
+      </c>
+      <c r="C83" s="2">
+        <v>134.22999999999999</v>
+      </c>
+      <c r="G83" s="1">
+        <v>500000</v>
+      </c>
+      <c r="H83">
+        <v>0.37046000000000001</v>
+      </c>
+      <c r="I83">
+        <v>0.12266000000000001</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="B84" s="2">
+        <v>66.424999999999997</v>
+      </c>
+      <c r="C84" s="2">
+        <v>267.81</v>
+      </c>
+      <c r="G84" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="H84">
+        <v>0.73397000000000001</v>
+      </c>
+      <c r="I84">
+        <v>0.25130999999999998</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>